<commit_message>
Imagen 11 para ficha del docente rec180
rec180
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion01/SolicitudGraficaMA_11_01_COREC180.xlsx
+++ b/fuentes/contenidos/grado11/guion01/SolicitudGraficaMA_11_01_COREC180.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="199">
   <si>
     <t>Fecha:</t>
   </si>
@@ -618,6 +618,12 @@
   </si>
   <si>
     <t>Imagen de ambientación</t>
+  </si>
+  <si>
+    <t>Función valor absoluto</t>
+  </si>
+  <si>
+    <t>Esta imagen es para una ficha del docente. Por favor ajustar par que su tamaño sea máximode 4cm por 4cm</t>
   </si>
 </sst>
 </file>
@@ -2194,6 +2200,44 @@
         <a:xfrm>
           <a:off x="13835063" y="8798718"/>
           <a:ext cx="4542553" cy="1000125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>440531</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>107156</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2678905</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>1572758</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14132719" y="19478625"/>
+          <a:ext cx="2238374" cy="1465602"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2922,7 +2966,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="D1" zoomScale="80" zoomScaleNormal="50" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J24" sqref="J24"/>
+      <selection pane="bottomLeft" activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3630,36 +3674,46 @@
         <v>F10</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" s="11" customFormat="1" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="B20" s="62"/>
+        <v>IMG11</v>
+      </c>
+      <c r="B20" s="62" t="s">
+        <v>188</v>
+      </c>
       <c r="C20" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D20" s="63"/>
-      <c r="E20" s="63"/>
+        <v>Recurso F6</v>
+      </c>
+      <c r="D20" s="63" t="s">
+        <v>189</v>
+      </c>
+      <c r="E20" s="63" t="s">
+        <v>155</v>
+      </c>
       <c r="F20" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" ca="1" si="4"/>
+        <v>MA_11_01_REC180_IMG11n.jpg</v>
       </c>
       <c r="G20" s="13" t="str">
         <f ca="1">IF($F20&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E20,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>320 x 480 px</v>
       </c>
       <c r="H20" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>MA_11_01_REC180_IMG11a.jpg</v>
       </c>
       <c r="I20" s="13" t="str">
         <f ca="1">IF(OR($B20&lt;&gt;"",$J20&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E20,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E20,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v/>
-      </c>
-      <c r="J20" s="64"/>
-      <c r="K20" s="66"/>
+        <v>800 x 458 px</v>
+      </c>
+      <c r="J20" s="64" t="s">
+        <v>197</v>
+      </c>
+      <c r="K20" s="66" t="s">
+        <v>198</v>
+      </c>
       <c r="O20" s="2" t="str">
         <f>'Definición técnica de imagenes'!A32</f>
         <v>F10B</v>

</xml_diff>